<commit_message>
Resize print area and data validation
</commit_message>
<xml_diff>
--- a/src/zxxt_02_excel_xlsx.w3mi.data.xlsx
+++ b/src/zxxt_02_excel_xlsx.w3mi.data.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Desktop\xtt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40503C2F-DE9D-4C26-8C94-FBD3E98B7B15}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$9</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
@@ -606,7 +610,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -633,6 +637,16 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -698,14 +712,14 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -735,14 +749,14 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -854,14 +868,15 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -890,22 +905,27 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1009,19 +1029,15 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
+        <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1153,11 +1169,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A3:E5" totalsRowCount="1" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A3:E4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Caption" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Group" dataDxfId="8" totalsRowDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Date" dataDxfId="7" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SUM1" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SUM2" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Caption" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Group" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Date" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SUM1" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SUM2" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1462,13 +1478,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="16.7109375" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="11" customWidth="1"/>
     <col min="4" max="5" width="16.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1487,7 +1504,7 @@
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -1504,7 +1521,7 @@
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -1519,7 +1536,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="10">
         <f>SUBTOTAL(109,Table2[SUM1])</f>
         <v>0</v>
@@ -1530,6 +1547,16 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:E4" xr:uid="{06600906-E9B7-4EBE-BC11-F86CBDFBC778}">
+      <formula1>0</formula1>
+      <formula2>1000000</formula2>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{8C9B6755-B171-4A99-BC56-60A16E28DCAA}">
+      <formula1>NOW()-3</formula1>
+      <formula2>NOW()+3</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>